<commit_message>
calibration sucess for pc commit
</commit_message>
<xml_diff>
--- a/data/output/PC/calibration/PC_Parameters.xlsx
+++ b/data/output/PC/calibration/PC_Parameters.xlsx
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2612.858772277832</v>
+        <v>2566.230922937393</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>949.2221393782385</v>
+        <v>947.796802961918</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>19.41181950947635</v>
+        <v>19.0594720423922</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>217.238347150259</v>
+        <v>216.3750789844852</v>
       </c>
     </row>
     <row r="8">

</xml_diff>